<commit_message>
units and components costs
</commit_message>
<xml_diff>
--- a/uploads/БАШ_НИПИ_новая_форма.xlsx
+++ b/uploads/БАШ_НИПИ_новая_форма.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aleksei\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B85D8DAD-6EEF-4ABA-96D4-E1ADC13A47F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B63CCDC-C88C-4B76-8DD3-9254CC95114B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
+    <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="39">
   <si>
     <t>Условное название</t>
   </si>
@@ -140,6 +141,9 @@
   </si>
   <si>
     <t>Базовой раствор №2 - средние значения</t>
+  </si>
+  <si>
+    <t>ед. из.</t>
   </si>
 </sst>
 </file>
@@ -484,8 +488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:X2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1610,7 +1614,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1676,4 +1680,155 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9F048BF-65D7-493B-83D7-1E2AF307B637}">
+  <dimension ref="A1:V2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P7" sqref="P7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:22" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="U2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="V2" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>